<commit_message>
Scroll adicionado as movimentações.
</commit_message>
<xml_diff>
--- a/PlanilhaMovs.xlsx
+++ b/PlanilhaMovs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,6 +557,108 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>R$ 1664.50</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Colégio</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Gasto</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>R$ 300</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Academia</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Gasto</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>R$ 709.33</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mercado</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Gasto</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>R$ 1500</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Plano de saúde</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Gasto</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>R$ 2000</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Aportes</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Gasto</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>R$ 1855.70</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Cartão</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Gasto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Alterações na planilha teste.
</commit_message>
<xml_diff>
--- a/PlanilhaMovs.xlsx
+++ b/PlanilhaMovs.xlsx
@@ -475,7 +475,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>R$ 400</t>
+          <t>R$ 400.00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -611,7 +611,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>R$ 1500</t>
+          <t>R$ 1500.00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>R$ 2000</t>
+          <t>R$ 2000.00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">

</xml_diff>